<commit_message>
CIS Update April 1 - May 1
</commit_message>
<xml_diff>
--- a/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Flag Updates.xlsx
+++ b/Tile Cal CIS Calib/CIS Updates/2022 2023 Jacky & Peter/Flag Updates.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter Camporeale\Documents\Research\CERN ATLAS 2022-2023\Tile-CIS-group\Tile Cal CIS Calib\CIS Updates\2022 2023 Jacky &amp; Peter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F46EF2-D3CD-4494-AC6D-7ACCE3456708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FAEF31-9E53-4641-ACCE-A1A41A0FFF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="15150" xr2:uid="{51C3CB71-5024-4996-BCC0-478F61F63DFE}"/>
   </bookViews>
   <sheets>
-    <sheet name="March 2023" sheetId="5" r:id="rId1"/>
-    <sheet name="February 2023" sheetId="4" r:id="rId2"/>
-    <sheet name="November 2022" sheetId="3" r:id="rId3"/>
-    <sheet name="September 2022" sheetId="2" r:id="rId4"/>
-    <sheet name="August 2022" sheetId="1" r:id="rId5"/>
+    <sheet name="April 2023" sheetId="6" r:id="rId1"/>
+    <sheet name="March 2023" sheetId="5" r:id="rId2"/>
+    <sheet name="February 2023" sheetId="4" r:id="rId3"/>
+    <sheet name="November 2022" sheetId="3" r:id="rId4"/>
+    <sheet name="September 2022" sheetId="2" r:id="rId5"/>
+    <sheet name="August 2022" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>Mark as Good (Remove BadCIS)</t>
   </si>
@@ -150,6 +151,15 @@
   </si>
   <si>
     <t>EBC_m23_c31_lowgain</t>
+  </si>
+  <si>
+    <t>EBA_m05_c10_lowgain</t>
+  </si>
+  <si>
+    <t>EBA_m09_c16_lowgain</t>
+  </si>
+  <si>
+    <t>EBA_m13_c04_lowgain</t>
   </si>
 </sst>
 </file>
@@ -608,19 +618,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389599CB-D1AF-423E-A34D-E5EF30783F72}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAB1234-0E12-4592-AA2F-266CA644CC06}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.77734375" customWidth="1"/>
+    <col min="1" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -628,41 +638,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>34</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B3" s="12"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -671,6 +662,69 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389599CB-D1AF-423E-A34D-E5EF30783F72}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2244AC6-0EEC-40D3-A825-368340C2A85E}">
   <dimension ref="A1:B18"/>
   <sheetViews>
@@ -678,12 +732,12 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.77734375" customWidth="1"/>
+    <col min="1" max="2" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -691,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -699,7 +753,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
@@ -707,77 +761,77 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>29</v>
       </c>
@@ -788,7 +842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3722913E-365D-4262-BF4E-9ED732B4CE06}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -796,12 +850,12 @@
       <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -809,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -817,19 +871,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="8"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="4"/>
     </row>
@@ -839,7 +893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF2EE4E-03F0-4650-AC7A-607ACD11D978}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -847,12 +901,12 @@
       <selection activeCell="B6" sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="54" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -860,24 +914,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
@@ -887,7 +941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{121ECB9F-C056-4550-AEED-7C9D041BDFDD}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -895,12 +949,12 @@
       <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -916,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>

</xml_diff>